<commit_message>
Updated spreadsheet and presentation
</commit_message>
<xml_diff>
--- a/data_analysis.xlsx
+++ b/data_analysis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chris/projects/warby_parker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D321DAB-879C-0942-AD84-EFA99DABA9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C553FFBD-E247-544A-989A-64F4F9036DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A15ABF3F-208A-664D-A0C8-DA459C8A87D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="95">
   <si>
     <t>question</t>
   </si>
@@ -318,13 +318,16 @@
   </si>
   <si>
     <t>Rows: 1000</t>
+  </si>
+  <si>
+    <t>Retention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +355,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -373,12 +382,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,14 +728,16 @@
   <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -847,12 +861,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="22" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -862,6 +879,9 @@
       <c r="B13" s="2">
         <v>500</v>
       </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -870,6 +890,10 @@
       <c r="B14" s="2">
         <v>475</v>
       </c>
+      <c r="C14" s="6">
+        <f>B14/B13</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -878,6 +902,10 @@
       <c r="B15" s="2">
         <v>380</v>
       </c>
+      <c r="C15" s="6">
+        <f t="shared" ref="C15:C17" si="0">B15/B14</f>
+        <v>0.8</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -886,6 +914,10 @@
       <c r="B16" s="2">
         <v>361</v>
       </c>
+      <c r="C16" s="6">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -894,6 +926,10 @@
       <c r="B17" s="2">
         <v>270</v>
       </c>
+      <c r="C17" s="6">
+        <f t="shared" si="0"/>
+        <v>0.74792243767313016</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -1340,11 +1376,11 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <v>75</v>
-      </c>
-      <c r="B48" s="2">
-        <v>66</v>
+      <c r="A48" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="B48" s="7">
+        <v>0.66</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -1359,16 +1395,16 @@
       <c r="A50" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="2">
-        <v>53.03</v>
+      <c r="B50" s="7">
+        <v>0.53029999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="2">
-        <v>79.25</v>
+      <c r="B51" s="7">
+        <v>0.79249999999999998</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">

</xml_diff>